<commit_message>
Reorganization of files, placement of currently unused files in "old" directories, and addition of pie charts used in figures to graphics rmd.
</commit_message>
<xml_diff>
--- a/documents/specimen_data.xlsx
+++ b/documents/specimen_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkam\Documents\Guadua_leaf_project\guadua_leaf\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723E2479-149E-4F6C-884F-C18421DAAE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476E805B-83D9-44B0-A1A3-E7E562F6F794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="1230" windowWidth="21360" windowHeight="14175" xr2:uid="{BD6EB2E0-2002-4F5B-817A-69EA751A87C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD6EB2E0-2002-4F5B-817A-69EA751A87C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,15 +753,9 @@
     <t>Clark_and_Oliveira_914</t>
   </si>
   <si>
-    <t>COL</t>
-  </si>
-  <si>
     <t>JAC</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -840,9 +834,6 @@
     <t>Cortes_26</t>
   </si>
   <si>
-    <t>G_tuxlensis</t>
-  </si>
-  <si>
     <t>Santos_3301</t>
   </si>
   <si>
@@ -871,6 +862,15 @@
   </si>
   <si>
     <t>Unknown_G_aff_sarcocarpa</t>
+  </si>
+  <si>
+    <t>G_refracta</t>
+  </si>
+  <si>
+    <t>G_guzmanii</t>
+  </si>
+  <si>
+    <t>G_tuxtlensis</t>
   </si>
 </sst>
 </file>
@@ -886,18 +886,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -912,10 +906,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1233,8 +1225,8 @@
   <dimension ref="A1:P190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B173" sqref="B173"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1595,7 @@
         <v>127</v>
       </c>
       <c r="P7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1653,7 +1645,7 @@
         <v>127</v>
       </c>
       <c r="P8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1753,7 +1745,7 @@
         <v>127</v>
       </c>
       <c r="P10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1803,7 +1795,7 @@
         <v>127</v>
       </c>
       <c r="P11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1876,7 +1868,7 @@
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
         <v>220</v>
@@ -1903,7 +1895,7 @@
         <v>127</v>
       </c>
       <c r="P13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1926,7 +1918,7 @@
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H14" t="s">
         <v>220</v>
@@ -1976,7 +1968,7 @@
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H15" t="s">
         <v>220</v>
@@ -2026,7 +2018,7 @@
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H16" t="s">
         <v>220</v>
@@ -2076,7 +2068,7 @@
         <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H17" t="s">
         <v>224</v>
@@ -2126,7 +2118,7 @@
         <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H18" t="s">
         <v>220</v>
@@ -2176,7 +2168,7 @@
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s">
         <v>220</v>
@@ -2226,7 +2218,7 @@
         <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H20" t="s">
         <v>220</v>
@@ -2253,7 +2245,7 @@
         <v>117</v>
       </c>
       <c r="P20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2276,7 +2268,7 @@
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H21" t="s">
         <v>220</v>
@@ -2303,7 +2295,7 @@
         <v>117</v>
       </c>
       <c r="P21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2326,7 +2318,7 @@
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H22" t="s">
         <v>220</v>
@@ -2353,7 +2345,7 @@
         <v>117</v>
       </c>
       <c r="P22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2376,7 +2368,7 @@
         <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H23" t="s">
         <v>224</v>
@@ -2453,7 +2445,7 @@
         <v>127</v>
       </c>
       <c r="P24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2529,7 +2521,7 @@
         <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="I26" t="s">
         <v>228</v>
@@ -2606,103 +2598,103 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" t="s">
         <v>224</v>
       </c>
       <c r="I28" t="s">
         <v>228</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" t="s">
         <v>232</v>
       </c>
       <c r="K28" t="s">
         <v>225</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="L28" t="s">
         <v>117</v>
       </c>
       <c r="M28" t="s">
         <v>229</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="N28" t="s">
+        <v>117</v>
+      </c>
+      <c r="O28" t="s">
+        <v>127</v>
+      </c>
+      <c r="P28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" t="s">
         <v>224</v>
       </c>
       <c r="I29" t="s">
         <v>228</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" t="s">
         <v>232</v>
       </c>
       <c r="K29" t="s">
         <v>225</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="L29" t="s">
         <v>117</v>
       </c>
       <c r="M29" t="s">
         <v>229</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P29" s="1" t="s">
+      <c r="N29" t="s">
+        <v>117</v>
+      </c>
+      <c r="O29" t="s">
+        <v>127</v>
+      </c>
+      <c r="P29" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2853,7 +2845,7 @@
         <v>127</v>
       </c>
       <c r="P32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2956,53 +2948,53 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" t="s">
         <v>10</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" t="s">
         <v>220</v>
       </c>
       <c r="I35" t="s">
         <v>228</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="K35" s="1" t="s">
+      <c r="J35" t="s">
+        <v>232</v>
+      </c>
+      <c r="K35" t="s">
         <v>225</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L35" t="s">
         <v>117</v>
       </c>
       <c r="M35" t="s">
         <v>229</v>
       </c>
-      <c r="N35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P35" s="1" t="s">
+      <c r="N35" t="s">
+        <v>117</v>
+      </c>
+      <c r="O35" t="s">
+        <v>127</v>
+      </c>
+      <c r="P35" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3376,7 +3368,7 @@
         <v>9</v>
       </c>
       <c r="G43" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H43" t="s">
         <v>220</v>
@@ -3403,7 +3395,7 @@
         <v>127</v>
       </c>
       <c r="P43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3426,7 +3418,7 @@
         <v>9</v>
       </c>
       <c r="G44" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H44" t="s">
         <v>220</v>
@@ -3476,7 +3468,7 @@
         <v>9</v>
       </c>
       <c r="G45" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H45" t="s">
         <v>224</v>
@@ -3526,7 +3518,7 @@
         <v>9</v>
       </c>
       <c r="G46" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H46" t="s">
         <v>224</v>
@@ -3576,7 +3568,7 @@
         <v>9</v>
       </c>
       <c r="G47" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H47" t="s">
         <v>220</v>
@@ -3626,7 +3618,7 @@
         <v>9</v>
       </c>
       <c r="G48" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H48" t="s">
         <v>220</v>
@@ -3658,7 +3650,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B49" t="s">
         <v>25</v>
@@ -3676,7 +3668,7 @@
         <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H49" t="s">
         <v>224</v>
@@ -3708,7 +3700,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
@@ -3717,7 +3709,7 @@
         <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E50" t="s">
         <v>22</v>
@@ -3726,7 +3718,7 @@
         <v>9</v>
       </c>
       <c r="G50" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H50" t="s">
         <v>224</v>
@@ -3758,10 +3750,10 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B51" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C51" t="s">
         <v>117</v>
@@ -3908,7 +3900,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B54" t="s">
         <v>28</v>
@@ -4003,7 +3995,7 @@
         <v>127</v>
       </c>
       <c r="P55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -4153,12 +4145,12 @@
         <v>127</v>
       </c>
       <c r="P58" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B59" t="s">
         <v>28</v>
@@ -4208,7 +4200,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
@@ -4458,7 +4450,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B65" t="s">
         <v>31</v>
@@ -4553,83 +4545,83 @@
         <v>127</v>
       </c>
       <c r="P66" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>280</v>
       </c>
       <c r="C67" t="s">
         <v>117</v>
       </c>
       <c r="D67" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G67" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H67" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I67" t="s">
         <v>228</v>
       </c>
       <c r="J67" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K67" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="L67" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M67" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N67" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="O67" t="s">
         <v>127</v>
       </c>
       <c r="P67" t="s">
-        <v>243</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>257</v>
+        <v>130</v>
       </c>
       <c r="B68" t="s">
-        <v>32</v>
+        <v>280</v>
       </c>
       <c r="C68" t="s">
         <v>117</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E68" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F68" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G68" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H68" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I68" t="s">
         <v>228</v>
@@ -4638,13 +4630,13 @@
         <v>232</v>
       </c>
       <c r="K68" t="s">
-        <v>256</v>
+        <v>127</v>
       </c>
       <c r="L68" t="s">
         <v>117</v>
       </c>
       <c r="M68" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="N68" t="s">
         <v>117</v>
@@ -4658,25 +4650,25 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C69" t="s">
         <v>117</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F69" t="s">
         <v>9</v>
       </c>
       <c r="G69" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="H69" t="s">
         <v>220</v>
@@ -4697,68 +4689,68 @@
         <v>230</v>
       </c>
       <c r="N69" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="O69" t="s">
         <v>127</v>
       </c>
       <c r="P69" t="s">
-        <v>127</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>255</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C70" t="s">
         <v>117</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E70" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F70" t="s">
         <v>9</v>
       </c>
       <c r="G70" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="H70" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I70" t="s">
         <v>228</v>
       </c>
       <c r="J70" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K70" t="s">
-        <v>127</v>
+        <v>254</v>
       </c>
       <c r="L70" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M70" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N70" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="O70" t="s">
         <v>127</v>
       </c>
       <c r="P70" t="s">
-        <v>243</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>258</v>
+        <v>109</v>
       </c>
       <c r="B71" t="s">
         <v>33</v>
@@ -4779,7 +4771,7 @@
         <v>29</v>
       </c>
       <c r="H71" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I71" t="s">
         <v>228</v>
@@ -4808,7 +4800,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B72" t="s">
         <v>33</v>
@@ -4829,7 +4821,7 @@
         <v>29</v>
       </c>
       <c r="H72" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I72" t="s">
         <v>228</v>
@@ -4853,112 +4845,112 @@
         <v>127</v>
       </c>
       <c r="P72" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>256</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C73" t="s">
         <v>117</v>
       </c>
       <c r="D73" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G73" t="s">
         <v>29</v>
       </c>
       <c r="H73" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I73" t="s">
         <v>228</v>
       </c>
       <c r="J73" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K73" t="s">
         <v>127</v>
       </c>
       <c r="L73" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M73" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N73" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O73" t="s">
         <v>127</v>
       </c>
       <c r="P73" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C74" t="s">
         <v>117</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G74" t="s">
         <v>29</v>
       </c>
       <c r="H74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I74" t="s">
         <v>228</v>
       </c>
       <c r="J74" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K74" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L74" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M74" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N74" t="s">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="O74" t="s">
         <v>127</v>
       </c>
       <c r="P74" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B75" t="s">
         <v>34</v>
@@ -5008,13 +5000,13 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B76" t="s">
         <v>34</v>
       </c>
       <c r="C76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D76" t="s">
         <v>6</v>
@@ -5058,7 +5050,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
         <v>34</v>
@@ -5158,7 +5150,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B79" t="s">
         <v>34</v>
@@ -5229,7 +5221,7 @@
         <v>29</v>
       </c>
       <c r="H80" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I80" t="s">
         <v>228</v>
@@ -5253,7 +5245,7 @@
         <v>127</v>
       </c>
       <c r="P80" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -5353,7 +5345,7 @@
         <v>127</v>
       </c>
       <c r="P82" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -5535,7 +5527,7 @@
         <v>228</v>
       </c>
       <c r="J86" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K86" t="s">
         <v>127</v>
@@ -5606,103 +5598,103 @@
         <v>127</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>141</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>135</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D88" s="1" t="s">
+      <c r="C88" t="s">
+        <v>117</v>
+      </c>
+      <c r="D88" t="s">
         <v>11</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>7</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="F88" t="s">
         <v>35</v>
       </c>
-      <c r="G88" s="1" t="s">
+      <c r="G88" t="s">
         <v>10</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="H88" t="s">
         <v>220</v>
       </c>
       <c r="I88" t="s">
         <v>228</v>
       </c>
-      <c r="J88" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="K88" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L88" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="N88" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="O88" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="P88" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B89" s="2" t="s">
+      <c r="J88" t="s">
+        <v>232</v>
+      </c>
+      <c r="K88" t="s">
+        <v>127</v>
+      </c>
+      <c r="L88" t="s">
+        <v>117</v>
+      </c>
+      <c r="M88" t="s">
+        <v>234</v>
+      </c>
+      <c r="N88" t="s">
+        <v>117</v>
+      </c>
+      <c r="O88" t="s">
+        <v>127</v>
+      </c>
+      <c r="P88" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>258</v>
+      </c>
+      <c r="B89" t="s">
         <v>38</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D89" s="2" t="s">
+      <c r="C89" t="s">
+        <v>117</v>
+      </c>
+      <c r="D89" t="s">
         <v>19</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" t="s">
         <v>16</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" t="s">
         <v>24</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="G89" t="s">
         <v>29</v>
       </c>
-      <c r="H89" s="2" t="s">
+      <c r="H89" t="s">
         <v>224</v>
       </c>
-      <c r="I89" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J89" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="K89" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L89" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M89" s="2" t="s">
+      <c r="I89" t="s">
+        <v>228</v>
+      </c>
+      <c r="J89" t="s">
+        <v>228</v>
+      </c>
+      <c r="K89" t="s">
+        <v>127</v>
+      </c>
+      <c r="L89" t="s">
+        <v>127</v>
+      </c>
+      <c r="M89" t="s">
         <v>230</v>
       </c>
-      <c r="N89" s="2" t="s">
+      <c r="N89" t="s">
         <v>230</v>
       </c>
-      <c r="O89" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="P89" s="2" t="s">
+      <c r="O89" t="s">
+        <v>127</v>
+      </c>
+      <c r="P89" t="s">
         <v>127</v>
       </c>
     </row>
@@ -5753,7 +5745,7 @@
         <v>127</v>
       </c>
       <c r="P90" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -5958,7 +5950,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B95" t="s">
         <v>38</v>
@@ -6053,12 +6045,12 @@
         <v>127</v>
       </c>
       <c r="P96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B97" t="s">
         <v>39</v>
@@ -6108,7 +6100,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B98" t="s">
         <v>39</v>
@@ -6253,7 +6245,7 @@
         <v>127</v>
       </c>
       <c r="P100" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -6308,7 +6300,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>223</v>
       </c>
       <c r="B102" t="s">
         <v>41</v>
@@ -6317,10 +6309,10 @@
         <v>117</v>
       </c>
       <c r="D102" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E102" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F102" t="s">
         <v>35</v>
@@ -6329,36 +6321,36 @@
         <v>42</v>
       </c>
       <c r="H102" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I102" t="s">
         <v>228</v>
       </c>
       <c r="J102" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K102" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="L102" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M102" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="N102" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O102" t="s">
         <v>127</v>
       </c>
       <c r="P102" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>223</v>
+        <v>151</v>
       </c>
       <c r="B103" t="s">
         <v>41</v>
@@ -6367,10 +6359,10 @@
         <v>117</v>
       </c>
       <c r="D103" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E103" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F103" t="s">
         <v>35</v>
@@ -6385,30 +6377,30 @@
         <v>228</v>
       </c>
       <c r="J103" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K103" t="s">
         <v>225</v>
       </c>
       <c r="L103" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M103" t="s">
         <v>229</v>
       </c>
       <c r="N103" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O103" t="s">
         <v>127</v>
       </c>
       <c r="P103" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B104" t="s">
         <v>41</v>
@@ -6458,7 +6450,7 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B105" t="s">
         <v>41</v>
@@ -6467,10 +6459,10 @@
         <v>117</v>
       </c>
       <c r="D105" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="E105" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F105" t="s">
         <v>35</v>
@@ -6485,30 +6477,30 @@
         <v>228</v>
       </c>
       <c r="J105" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K105" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L105" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M105" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N105" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O105" t="s">
         <v>127</v>
       </c>
       <c r="P105" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B106" t="s">
         <v>41</v>
@@ -6517,10 +6509,10 @@
         <v>117</v>
       </c>
       <c r="D106" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="E106" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F106" t="s">
         <v>35</v>
@@ -6535,30 +6527,30 @@
         <v>228</v>
       </c>
       <c r="J106" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K106" t="s">
         <v>127</v>
       </c>
       <c r="L106" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M106" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N106" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O106" t="s">
         <v>127</v>
       </c>
       <c r="P106" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B107" t="s">
         <v>41</v>
@@ -6567,7 +6559,7 @@
         <v>117</v>
       </c>
       <c r="D107" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E107" t="s">
         <v>22</v>
@@ -6579,7 +6571,7 @@
         <v>42</v>
       </c>
       <c r="H107" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I107" t="s">
         <v>228</v>
@@ -6588,13 +6580,13 @@
         <v>232</v>
       </c>
       <c r="K107" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="L107" t="s">
         <v>117</v>
       </c>
       <c r="M107" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N107" t="s">
         <v>117</v>
@@ -6608,7 +6600,7 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B108" t="s">
         <v>41</v>
@@ -6617,7 +6609,7 @@
         <v>117</v>
       </c>
       <c r="D108" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E108" t="s">
         <v>22</v>
@@ -6658,7 +6650,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B109" t="s">
         <v>41</v>
@@ -6667,10 +6659,10 @@
         <v>117</v>
       </c>
       <c r="D109" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E109" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F109" t="s">
         <v>35</v>
@@ -6679,7 +6671,7 @@
         <v>42</v>
       </c>
       <c r="H109" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I109" t="s">
         <v>228</v>
@@ -6688,13 +6680,13 @@
         <v>232</v>
       </c>
       <c r="K109" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="L109" t="s">
         <v>117</v>
       </c>
       <c r="M109" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N109" t="s">
         <v>117</v>
@@ -6708,7 +6700,7 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>157</v>
+        <v>262</v>
       </c>
       <c r="B110" t="s">
         <v>41</v>
@@ -6717,10 +6709,10 @@
         <v>117</v>
       </c>
       <c r="D110" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E110" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F110" t="s">
         <v>35</v>
@@ -6729,7 +6721,7 @@
         <v>42</v>
       </c>
       <c r="H110" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I110" t="s">
         <v>228</v>
@@ -6758,7 +6750,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>158</v>
+        <v>263</v>
       </c>
       <c r="B111" t="s">
         <v>41</v>
@@ -6779,7 +6771,7 @@
         <v>42</v>
       </c>
       <c r="H111" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I111" t="s">
         <v>228</v>
@@ -6803,12 +6795,12 @@
         <v>127</v>
       </c>
       <c r="P111" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B112" t="s">
         <v>41</v>
@@ -6817,10 +6809,10 @@
         <v>117</v>
       </c>
       <c r="D112" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E112" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F112" t="s">
         <v>35</v>
@@ -6829,7 +6821,7 @@
         <v>42</v>
       </c>
       <c r="H112" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I112" t="s">
         <v>228</v>
@@ -6858,7 +6850,7 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B113" t="s">
         <v>41</v>
@@ -6867,10 +6859,10 @@
         <v>117</v>
       </c>
       <c r="D113" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E113" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F113" t="s">
         <v>35</v>
@@ -6885,30 +6877,30 @@
         <v>228</v>
       </c>
       <c r="J113" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K113" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="L113" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M113" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="N113" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O113" t="s">
         <v>127</v>
       </c>
       <c r="P113" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B114" t="s">
         <v>41</v>
@@ -6917,10 +6909,10 @@
         <v>117</v>
       </c>
       <c r="D114" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E114" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F114" t="s">
         <v>35</v>
@@ -6929,7 +6921,7 @@
         <v>42</v>
       </c>
       <c r="H114" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I114" t="s">
         <v>228</v>
@@ -6958,7 +6950,7 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>264</v>
+        <v>166</v>
       </c>
       <c r="B115" t="s">
         <v>41</v>
@@ -6967,10 +6959,10 @@
         <v>117</v>
       </c>
       <c r="D115" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="E115" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F115" t="s">
         <v>35</v>
@@ -6979,36 +6971,36 @@
         <v>42</v>
       </c>
       <c r="H115" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I115" t="s">
         <v>228</v>
       </c>
       <c r="J115" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K115" t="s">
         <v>127</v>
       </c>
       <c r="L115" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M115" t="s">
+        <v>234</v>
+      </c>
+      <c r="N115" t="s">
         <v>230</v>
       </c>
-      <c r="N115" t="s">
-        <v>117</v>
-      </c>
       <c r="O115" t="s">
         <v>127</v>
       </c>
       <c r="P115" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
       <c r="B116" t="s">
         <v>41</v>
@@ -7017,10 +7009,10 @@
         <v>117</v>
       </c>
       <c r="D116" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E116" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F116" t="s">
         <v>35</v>
@@ -7029,28 +7021,28 @@
         <v>42</v>
       </c>
       <c r="H116" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I116" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="J116" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K116" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="L116" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M116" t="s">
+        <v>117</v>
+      </c>
+      <c r="N116" t="s">
         <v>230</v>
       </c>
-      <c r="N116" t="s">
-        <v>117</v>
-      </c>
       <c r="O116" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="P116" t="s">
         <v>127</v>
@@ -7058,7 +7050,7 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B117" t="s">
         <v>41</v>
@@ -7067,7 +7059,7 @@
         <v>117</v>
       </c>
       <c r="D117" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="E117" t="s">
         <v>7</v>
@@ -7085,48 +7077,48 @@
         <v>228</v>
       </c>
       <c r="J117" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K117" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L117" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M117" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N117" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O117" t="s">
         <v>127</v>
       </c>
       <c r="P117" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B118" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C118" t="s">
         <v>117</v>
       </c>
       <c r="D118" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E118" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F118" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G118" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H118" t="s">
         <v>220</v>
@@ -7135,48 +7127,48 @@
         <v>228</v>
       </c>
       <c r="J118" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K118" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L118" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M118" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N118" t="s">
-        <v>117</v>
+        <v>234</v>
       </c>
       <c r="O118" t="s">
         <v>127</v>
       </c>
       <c r="P118" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C119" t="s">
         <v>117</v>
       </c>
       <c r="D119" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E119" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F119" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G119" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H119" t="s">
         <v>220</v>
@@ -7188,13 +7180,13 @@
         <v>232</v>
       </c>
       <c r="K119" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L119" t="s">
         <v>117</v>
       </c>
       <c r="M119" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N119" t="s">
         <v>117</v>
@@ -7208,25 +7200,25 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B120" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C120" t="s">
         <v>117</v>
       </c>
       <c r="D120" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E120" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F120" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G120" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H120" t="s">
         <v>220</v>
@@ -7235,92 +7227,92 @@
         <v>228</v>
       </c>
       <c r="J120" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K120" t="s">
         <v>127</v>
       </c>
       <c r="L120" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M120" t="s">
         <v>234</v>
       </c>
       <c r="N120" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O120" t="s">
         <v>127</v>
       </c>
       <c r="P120" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
       <c r="B121" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C121" t="s">
         <v>117</v>
       </c>
       <c r="D121" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E121" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F121" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G121" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H121" t="s">
         <v>220</v>
       </c>
       <c r="I121" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J121" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K121" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="L121" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M121" t="s">
-        <v>117</v>
+        <v>229</v>
       </c>
       <c r="N121" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O121" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="P121" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B122" t="s">
-        <v>41</v>
+        <v>279</v>
       </c>
       <c r="C122" t="s">
         <v>117</v>
       </c>
       <c r="D122" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E122" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F122" t="s">
         <v>35</v>
@@ -7329,39 +7321,39 @@
         <v>42</v>
       </c>
       <c r="H122" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I122" t="s">
         <v>228</v>
       </c>
       <c r="J122" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K122" t="s">
         <v>127</v>
       </c>
       <c r="L122" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M122" t="s">
         <v>234</v>
       </c>
       <c r="N122" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O122" t="s">
         <v>127</v>
       </c>
       <c r="P122" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B123" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
       <c r="C123" t="s">
         <v>117</v>
@@ -7373,10 +7365,10 @@
         <v>22</v>
       </c>
       <c r="F123" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G123" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H123" t="s">
         <v>220</v>
@@ -7385,48 +7377,48 @@
         <v>228</v>
       </c>
       <c r="J123" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K123" t="s">
         <v>127</v>
       </c>
       <c r="L123" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M123" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N123" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="O123" t="s">
         <v>127</v>
       </c>
       <c r="P123" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B124" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
       <c r="C124" t="s">
         <v>117</v>
       </c>
       <c r="D124" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E124" t="s">
         <v>22</v>
       </c>
       <c r="F124" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G124" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H124" t="s">
         <v>220</v>
@@ -7435,48 +7427,48 @@
         <v>228</v>
       </c>
       <c r="J124" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K124" t="s">
         <v>127</v>
       </c>
       <c r="L124" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M124" t="s">
         <v>234</v>
       </c>
       <c r="N124" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O124" t="s">
         <v>127</v>
       </c>
       <c r="P124" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B125" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
       <c r="C125" t="s">
         <v>117</v>
       </c>
       <c r="D125" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
       </c>
       <c r="F125" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G125" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H125" t="s">
         <v>220</v>
@@ -7494,7 +7486,7 @@
         <v>117</v>
       </c>
       <c r="M125" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N125" t="s">
         <v>117</v>
@@ -7508,28 +7500,28 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B126" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
       <c r="C126" t="s">
         <v>117</v>
       </c>
       <c r="D126" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E126" t="s">
         <v>22</v>
       </c>
       <c r="F126" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="G126" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H126" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="I126" t="s">
         <v>228</v>
@@ -7538,13 +7530,13 @@
         <v>232</v>
       </c>
       <c r="K126" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L126" t="s">
         <v>117</v>
       </c>
       <c r="M126" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="N126" t="s">
         <v>117</v>
@@ -7608,7 +7600,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B128" t="s">
         <v>46</v>
@@ -7658,7 +7650,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B129" t="s">
         <v>46</v>
@@ -8258,7 +8250,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B141" t="s">
         <v>48</v>
@@ -8353,12 +8345,12 @@
         <v>127</v>
       </c>
       <c r="P142" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B143" t="s">
         <v>48</v>
@@ -8453,7 +8445,7 @@
         <v>117</v>
       </c>
       <c r="P144" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
@@ -8553,7 +8545,7 @@
         <v>127</v>
       </c>
       <c r="P146" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
@@ -8603,7 +8595,7 @@
         <v>117</v>
       </c>
       <c r="P147" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
@@ -8853,7 +8845,7 @@
         <v>127</v>
       </c>
       <c r="P152" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
@@ -8908,10 +8900,10 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B154" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="C154" t="s">
         <v>117</v>
@@ -9103,7 +9095,7 @@
         <v>127</v>
       </c>
       <c r="P157" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
@@ -9126,7 +9118,7 @@
         <v>9</v>
       </c>
       <c r="G158" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H158" t="s">
         <v>220</v>
@@ -9176,7 +9168,7 @@
         <v>9</v>
       </c>
       <c r="G159" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H159" t="s">
         <v>220</v>
@@ -9226,7 +9218,7 @@
         <v>9</v>
       </c>
       <c r="G160" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H160" t="s">
         <v>224</v>
@@ -9276,7 +9268,7 @@
         <v>9</v>
       </c>
       <c r="G161" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H161" t="s">
         <v>220</v>
@@ -9326,7 +9318,7 @@
         <v>9</v>
       </c>
       <c r="G162" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H162" t="s">
         <v>224</v>
@@ -9358,7 +9350,7 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B163" t="s">
         <v>51</v>
@@ -9376,7 +9368,7 @@
         <v>9</v>
       </c>
       <c r="G163" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H163" t="s">
         <v>224</v>
@@ -9426,7 +9418,7 @@
         <v>9</v>
       </c>
       <c r="G164" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H164" t="s">
         <v>224</v>
@@ -9476,7 +9468,7 @@
         <v>9</v>
       </c>
       <c r="G165" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H165" t="s">
         <v>224</v>
@@ -9508,7 +9500,7 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B166" t="s">
         <v>52</v>
@@ -9653,7 +9645,7 @@
         <v>127</v>
       </c>
       <c r="P168" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.25">
@@ -9703,12 +9695,12 @@
         <v>127</v>
       </c>
       <c r="P169" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B170" t="s">
         <v>52</v>
@@ -9758,7 +9750,7 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B171" t="s">
         <v>52</v>
@@ -9858,7 +9850,7 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B173" t="s">
         <v>52</v>
@@ -9958,7 +9950,7 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B175" t="s">
         <v>53</v>
@@ -10153,12 +10145,12 @@
         <v>127</v>
       </c>
       <c r="P178" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B179" t="s">
         <v>54</v>
@@ -10308,7 +10300,7 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B182" t="s">
         <v>54</v>
@@ -10558,10 +10550,10 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B187" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C187" t="s">
         <v>117</v>
@@ -10572,7 +10564,7 @@
       <c r="E187" t="s">
         <v>22</v>
       </c>
-      <c r="F187" s="2" t="s">
+      <c r="F187" t="s">
         <v>24</v>
       </c>
       <c r="G187" t="s">
@@ -10726,7 +10718,7 @@
         <v>24</v>
       </c>
       <c r="G190" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H190" t="s">
         <v>220</v>
@@ -10753,10 +10745,13 @@
         <v>127</v>
       </c>
       <c r="P190" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P190">
+    <sortCondition ref="B2:B190"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Edits to micromorphological analysis and graphics to reflect splitting of forest and river habitats.
</commit_message>
<xml_diff>
--- a/documents/specimen_data.xlsx
+++ b/documents/specimen_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkam\Documents\Guadua_leaf_project\guadua_leaf\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476E805B-83D9-44B0-A1A3-E7E562F6F794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FA30E-D55C-4673-A8D5-32A07C914F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD6EB2E0-2002-4F5B-817A-69EA751A87C6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3040" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3056" uniqueCount="281">
   <si>
     <t>Specimen</t>
   </si>
@@ -756,9 +756,6 @@
     <t>JAC</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -789,9 +786,6 @@
     <t>McDaniel_et_al_24883</t>
   </si>
   <si>
-    <t>EKm</t>
-  </si>
-  <si>
     <t>Londono_and_Quintero_214</t>
   </si>
   <si>
@@ -871,6 +865,9 @@
   </si>
   <si>
     <t>G_tuxtlensis</t>
+  </si>
+  <si>
+    <t>Nelson_6026</t>
   </si>
 </sst>
 </file>
@@ -1222,11 +1219,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B56512-CAAA-43F2-BB91-3587863148F1}">
-  <dimension ref="A1:P190"/>
+  <dimension ref="A1:P191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="2" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I134" sqref="I134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3650,7 +3647,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B49" t="s">
         <v>25</v>
@@ -3700,7 +3697,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
@@ -3709,7 +3706,7 @@
         <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E50" t="s">
         <v>22</v>
@@ -3750,10 +3747,10 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>247</v>
+      </c>
+      <c r="B51" t="s">
         <v>248</v>
-      </c>
-      <c r="B51" t="s">
-        <v>249</v>
       </c>
       <c r="C51" t="s">
         <v>117</v>
@@ -3900,7 +3897,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B54" t="s">
         <v>28</v>
@@ -4150,7 +4147,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B59" t="s">
         <v>28</v>
@@ -4200,7 +4197,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
@@ -4450,7 +4447,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B65" t="s">
         <v>31</v>
@@ -4553,7 +4550,7 @@
         <v>113</v>
       </c>
       <c r="B67" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C67" t="s">
         <v>117</v>
@@ -4603,7 +4600,7 @@
         <v>130</v>
       </c>
       <c r="B68" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C68" t="s">
         <v>117</v>
@@ -4700,7 +4697,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B70" t="s">
         <v>32</v>
@@ -4730,7 +4727,7 @@
         <v>232</v>
       </c>
       <c r="K70" t="s">
-        <v>254</v>
+        <v>127</v>
       </c>
       <c r="L70" t="s">
         <v>117</v>
@@ -4850,7 +4847,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B73" t="s">
         <v>33</v>
@@ -5150,7 +5147,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B79" t="s">
         <v>34</v>
@@ -5221,7 +5218,7 @@
         <v>29</v>
       </c>
       <c r="H80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I80" t="s">
         <v>228</v>
@@ -5527,7 +5524,7 @@
         <v>228</v>
       </c>
       <c r="J86" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="K86" t="s">
         <v>127</v>
@@ -5650,7 +5647,7 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B89" t="s">
         <v>38</v>
@@ -5950,7 +5947,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B95" t="s">
         <v>38</v>
@@ -6050,7 +6047,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B97" t="s">
         <v>39</v>
@@ -6100,7 +6097,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B98" t="s">
         <v>39</v>
@@ -6700,7 +6697,7 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B110" t="s">
         <v>41</v>
@@ -6750,7 +6747,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B111" t="s">
         <v>41</v>
@@ -7303,7 +7300,7 @@
         <v>150</v>
       </c>
       <c r="B122" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C122" t="s">
         <v>117</v>
@@ -7353,7 +7350,7 @@
         <v>154</v>
       </c>
       <c r="B123" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C123" t="s">
         <v>117</v>
@@ -7403,7 +7400,7 @@
         <v>155</v>
       </c>
       <c r="B124" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C124" t="s">
         <v>117</v>
@@ -7453,7 +7450,7 @@
         <v>157</v>
       </c>
       <c r="B125" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C125" t="s">
         <v>117</v>
@@ -7503,7 +7500,7 @@
         <v>158</v>
       </c>
       <c r="B126" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C126" t="s">
         <v>117</v>
@@ -7600,7 +7597,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B128" t="s">
         <v>46</v>
@@ -7650,7 +7647,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B129" t="s">
         <v>46</v>
@@ -8250,7 +8247,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B141" t="s">
         <v>48</v>
@@ -8350,7 +8347,7 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B143" t="s">
         <v>48</v>
@@ -8477,7 +8474,7 @@
         <v>228</v>
       </c>
       <c r="J145" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
       <c r="K145" t="s">
         <v>225</v>
@@ -8900,10 +8897,10 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B154" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C154" t="s">
         <v>117</v>
@@ -9350,7 +9347,7 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B163" t="s">
         <v>51</v>
@@ -9500,7 +9497,7 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B166" t="s">
         <v>52</v>
@@ -9700,7 +9697,7 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B170" t="s">
         <v>52</v>
@@ -9750,7 +9747,7 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B171" t="s">
         <v>52</v>
@@ -9850,7 +9847,7 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B173" t="s">
         <v>52</v>
@@ -9950,7 +9947,7 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B175" t="s">
         <v>53</v>
@@ -10150,7 +10147,7 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B179" t="s">
         <v>54</v>
@@ -10300,7 +10297,7 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B182" t="s">
         <v>54</v>
@@ -10309,10 +10306,10 @@
         <v>117</v>
       </c>
       <c r="D182" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E182" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F182" t="s">
         <v>24</v>
@@ -10350,7 +10347,7 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>210</v>
+        <v>274</v>
       </c>
       <c r="B183" t="s">
         <v>54</v>
@@ -10371,36 +10368,36 @@
         <v>10</v>
       </c>
       <c r="H183" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I183" t="s">
         <v>228</v>
       </c>
       <c r="J183" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K183" t="s">
         <v>127</v>
       </c>
       <c r="L183" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M183" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N183" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O183" t="s">
         <v>127</v>
       </c>
       <c r="P183" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B184" t="s">
         <v>54</v>
@@ -10409,10 +10406,10 @@
         <v>117</v>
       </c>
       <c r="D184" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E184" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F184" t="s">
         <v>24</v>
@@ -10427,30 +10424,30 @@
         <v>228</v>
       </c>
       <c r="J184" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K184" t="s">
         <v>127</v>
       </c>
       <c r="L184" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M184" t="s">
         <v>234</v>
       </c>
       <c r="N184" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O184" t="s">
         <v>127</v>
       </c>
       <c r="P184" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B185" t="s">
         <v>54</v>
@@ -10459,10 +10456,10 @@
         <v>117</v>
       </c>
       <c r="D185" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E185" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F185" t="s">
         <v>24</v>
@@ -10471,57 +10468,57 @@
         <v>10</v>
       </c>
       <c r="H185" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I185" t="s">
         <v>228</v>
       </c>
       <c r="J185" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K185" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L185" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M185" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N185" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O185" t="s">
         <v>127</v>
       </c>
       <c r="P185" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B186" t="s">
-        <v>216</v>
+        <v>54</v>
       </c>
       <c r="C186" t="s">
         <v>117</v>
       </c>
       <c r="D186" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E186" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F186" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G186" t="s">
         <v>10</v>
       </c>
       <c r="H186" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="I186" t="s">
         <v>228</v>
@@ -10550,10 +10547,10 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>277</v>
+        <v>221</v>
       </c>
       <c r="B187" t="s">
-        <v>278</v>
+        <v>216</v>
       </c>
       <c r="C187" t="s">
         <v>117</v>
@@ -10565,7 +10562,7 @@
         <v>22</v>
       </c>
       <c r="F187" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="G187" t="s">
         <v>10</v>
@@ -10577,33 +10574,33 @@
         <v>228</v>
       </c>
       <c r="J187" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="K187" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="L187" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M187" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N187" t="s">
-        <v>230</v>
+        <v>117</v>
       </c>
       <c r="O187" t="s">
         <v>127</v>
       </c>
       <c r="P187" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>213</v>
+        <v>275</v>
       </c>
       <c r="B188" t="s">
-        <v>217</v>
+        <v>276</v>
       </c>
       <c r="C188" t="s">
         <v>117</v>
@@ -10615,7 +10612,7 @@
         <v>22</v>
       </c>
       <c r="F188" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="G188" t="s">
         <v>10</v>
@@ -10627,33 +10624,33 @@
         <v>228</v>
       </c>
       <c r="J188" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K188" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="L188" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="M188" t="s">
         <v>230</v>
       </c>
       <c r="N188" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="O188" t="s">
         <v>127</v>
       </c>
       <c r="P188" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B189" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C189" t="s">
         <v>117</v>
@@ -10668,7 +10665,7 @@
         <v>35</v>
       </c>
       <c r="G189" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H189" t="s">
         <v>220</v>
@@ -10680,13 +10677,13 @@
         <v>232</v>
       </c>
       <c r="K189" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="L189" t="s">
         <v>117</v>
       </c>
       <c r="M189" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="N189" t="s">
         <v>117</v>
@@ -10700,57 +10697,107 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B190" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C190" t="s">
         <v>117</v>
       </c>
       <c r="D190" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E190" t="s">
         <v>22</v>
       </c>
       <c r="F190" t="s">
+        <v>35</v>
+      </c>
+      <c r="G190" t="s">
+        <v>42</v>
+      </c>
+      <c r="H190" t="s">
+        <v>220</v>
+      </c>
+      <c r="I190" t="s">
+        <v>228</v>
+      </c>
+      <c r="J190" t="s">
+        <v>232</v>
+      </c>
+      <c r="K190" t="s">
+        <v>127</v>
+      </c>
+      <c r="L190" t="s">
+        <v>117</v>
+      </c>
+      <c r="M190" t="s">
+        <v>234</v>
+      </c>
+      <c r="N190" t="s">
+        <v>117</v>
+      </c>
+      <c r="O190" t="s">
+        <v>127</v>
+      </c>
+      <c r="P190" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>215</v>
+      </c>
+      <c r="B191" t="s">
+        <v>219</v>
+      </c>
+      <c r="C191" t="s">
+        <v>117</v>
+      </c>
+      <c r="D191" t="s">
+        <v>26</v>
+      </c>
+      <c r="E191" t="s">
+        <v>22</v>
+      </c>
+      <c r="F191" t="s">
         <v>24</v>
       </c>
-      <c r="G190" t="s">
+      <c r="G191" t="s">
         <v>29</v>
       </c>
-      <c r="H190" t="s">
-        <v>220</v>
-      </c>
-      <c r="I190" t="s">
-        <v>228</v>
-      </c>
-      <c r="J190" t="s">
-        <v>228</v>
-      </c>
-      <c r="K190" t="s">
-        <v>127</v>
-      </c>
-      <c r="L190" t="s">
-        <v>127</v>
-      </c>
-      <c r="M190" t="s">
-        <v>234</v>
-      </c>
-      <c r="N190" t="s">
-        <v>234</v>
-      </c>
-      <c r="O190" t="s">
-        <v>127</v>
-      </c>
-      <c r="P190" t="s">
+      <c r="H191" t="s">
+        <v>220</v>
+      </c>
+      <c r="I191" t="s">
+        <v>228</v>
+      </c>
+      <c r="J191" t="s">
+        <v>228</v>
+      </c>
+      <c r="K191" t="s">
+        <v>127</v>
+      </c>
+      <c r="L191" t="s">
+        <v>127</v>
+      </c>
+      <c r="M191" t="s">
+        <v>234</v>
+      </c>
+      <c r="N191" t="s">
+        <v>234</v>
+      </c>
+      <c r="O191" t="s">
+        <v>127</v>
+      </c>
+      <c r="P191" t="s">
         <v>242</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P190">
-    <sortCondition ref="B2:B190"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P191">
+    <sortCondition ref="B2:B191"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Removing files not currently in use and adding main README
</commit_message>
<xml_diff>
--- a/documents/specimen_data.xlsx
+++ b/documents/specimen_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elkam\Documents\Guadua_leaf_project\guadua_leaf\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FA30E-D55C-4673-A8D5-32A07C914F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989C61C2-058A-443D-9BDD-BA38992CEF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD6EB2E0-2002-4F5B-817A-69EA751A87C6}"/>
   </bookViews>
@@ -1222,8 +1222,8 @@
   <dimension ref="A1:P191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I134" sqref="I134"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>